<commit_message>
more plate from 0 to 1
</commit_message>
<xml_diff>
--- a/workflow-cgi/workflow-Genotype/0-scanner-labid/3000142572.xlsx
+++ b/workflow-cgi/workflow-Genotype/0-scanner-labid/3000142572.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thokall/Documents/SeqDB-documentation/workflow-cgi/workflow-Genotype/0-scanner-labid/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="460" windowWidth="24920" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +19,15 @@
   <definedNames>
     <definedName name="NRM_CGI_3000142572_20191210" localSheetId="0">Sheet1!$A$1:$D$97</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -333,9 +346,6 @@
     <t>H12</t>
   </si>
   <si>
-    <t>LabID</t>
-  </si>
-  <si>
     <t>S8</t>
   </si>
   <si>
@@ -622,6 +632,9 @@
   </si>
   <si>
     <t>S103</t>
+  </si>
+  <si>
+    <t>Lab ID</t>
   </si>
 </sst>
 </file>
@@ -720,12 +733,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -755,12 +768,12 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -966,17 +979,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A98" sqref="A98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -987,10 +1000,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1001,10 +1014,10 @@
         <v>3000142572</v>
       </c>
       <c r="D2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1015,10 +1028,10 @@
         <v>3000142572</v>
       </c>
       <c r="D3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -1029,10 +1042,10 @@
         <v>3000142572</v>
       </c>
       <c r="D4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1043,10 +1056,10 @@
         <v>3000142572</v>
       </c>
       <c r="D5" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1057,10 +1070,10 @@
         <v>3000142572</v>
       </c>
       <c r="D6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1071,10 +1084,10 @@
         <v>3000142572</v>
       </c>
       <c r="D7" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1085,10 +1098,10 @@
         <v>3000142572</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1099,10 +1112,10 @@
         <v>3000142572</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1113,10 +1126,10 @@
         <v>3000142572</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -1127,10 +1140,10 @@
         <v>3000142572</v>
       </c>
       <c r="D11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -1141,10 +1154,10 @@
         <v>3000142572</v>
       </c>
       <c r="D12" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -1155,10 +1168,10 @@
         <v>3000142572</v>
       </c>
       <c r="D13" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -1169,10 +1182,10 @@
         <v>3000142572</v>
       </c>
       <c r="D14" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -1183,10 +1196,10 @@
         <v>3000142572</v>
       </c>
       <c r="D15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1197,10 +1210,10 @@
         <v>3000142572</v>
       </c>
       <c r="D16" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -1211,10 +1224,10 @@
         <v>3000142572</v>
       </c>
       <c r="D17" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1225,10 +1238,10 @@
         <v>3000142572</v>
       </c>
       <c r="D18" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -1239,10 +1252,10 @@
         <v>3000142572</v>
       </c>
       <c r="D19" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -1253,10 +1266,10 @@
         <v>3000142572</v>
       </c>
       <c r="D20" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1267,10 +1280,10 @@
         <v>3000142572</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1281,10 +1294,10 @@
         <v>3000142572</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1295,10 +1308,10 @@
         <v>3000142572</v>
       </c>
       <c r="D23" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1309,10 +1322,10 @@
         <v>3000142572</v>
       </c>
       <c r="D24" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1323,10 +1336,10 @@
         <v>3000142572</v>
       </c>
       <c r="D25" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1337,10 +1350,10 @@
         <v>3000142572</v>
       </c>
       <c r="D26" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1351,10 +1364,10 @@
         <v>3000142572</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1365,10 +1378,10 @@
         <v>3000142572</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1379,10 +1392,10 @@
         <v>3000142572</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1393,10 +1406,10 @@
         <v>3000142572</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1407,10 +1420,10 @@
         <v>3000142572</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1421,10 +1434,10 @@
         <v>3000142572</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1435,10 +1448,10 @@
         <v>3000142572</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1449,10 +1462,10 @@
         <v>3000142572</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1463,10 +1476,10 @@
         <v>3000142572</v>
       </c>
       <c r="D35" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1477,10 +1490,10 @@
         <v>3000142572</v>
       </c>
       <c r="D36" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1491,10 +1504,10 @@
         <v>3000142572</v>
       </c>
       <c r="D37" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1505,10 +1518,10 @@
         <v>3000142572</v>
       </c>
       <c r="D38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1519,10 +1532,10 @@
         <v>3000142572</v>
       </c>
       <c r="D39" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1533,10 +1546,10 @@
         <v>3000142572</v>
       </c>
       <c r="D40" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1547,10 +1560,10 @@
         <v>3000142572</v>
       </c>
       <c r="D41" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1561,10 +1574,10 @@
         <v>3000142572</v>
       </c>
       <c r="D42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1575,10 +1588,10 @@
         <v>3000142572</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1589,10 +1602,10 @@
         <v>3000142572</v>
       </c>
       <c r="D44" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1603,10 +1616,10 @@
         <v>3000142572</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1617,10 +1630,10 @@
         <v>3000142572</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1631,10 +1644,10 @@
         <v>3000142572</v>
       </c>
       <c r="D47" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1645,10 +1658,10 @@
         <v>3000142572</v>
       </c>
       <c r="D48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1659,10 +1672,10 @@
         <v>3000142572</v>
       </c>
       <c r="D49" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1673,10 +1686,10 @@
         <v>3000142572</v>
       </c>
       <c r="D50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1687,10 +1700,10 @@
         <v>3000142572</v>
       </c>
       <c r="D51" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1701,10 +1714,10 @@
         <v>3000142572</v>
       </c>
       <c r="D52" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1715,10 +1728,10 @@
         <v>3000142572</v>
       </c>
       <c r="D53" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1729,10 +1742,10 @@
         <v>3000142572</v>
       </c>
       <c r="D54" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1743,10 +1756,10 @@
         <v>3000142572</v>
       </c>
       <c r="D55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1757,10 +1770,10 @@
         <v>3000142572</v>
       </c>
       <c r="D56" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1771,10 +1784,10 @@
         <v>3000142572</v>
       </c>
       <c r="D57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1785,10 +1798,10 @@
         <v>3000142572</v>
       </c>
       <c r="D58" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1799,10 +1812,10 @@
         <v>3000142572</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1813,10 +1826,10 @@
         <v>3000142572</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1827,10 +1840,10 @@
         <v>3000142572</v>
       </c>
       <c r="D61" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1841,10 +1854,10 @@
         <v>3000142572</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1855,10 +1868,10 @@
         <v>3000142572</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1869,10 +1882,10 @@
         <v>3000142572</v>
       </c>
       <c r="D64" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -1883,10 +1896,10 @@
         <v>3000142572</v>
       </c>
       <c r="D65" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -1897,10 +1910,10 @@
         <v>3000142572</v>
       </c>
       <c r="D66" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -1911,10 +1924,10 @@
         <v>3000142572</v>
       </c>
       <c r="D67" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>69</v>
       </c>
@@ -1925,10 +1938,10 @@
         <v>3000142572</v>
       </c>
       <c r="D68" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>70</v>
       </c>
@@ -1939,10 +1952,10 @@
         <v>3000142572</v>
       </c>
       <c r="D69" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>71</v>
       </c>
@@ -1953,10 +1966,10 @@
         <v>3000142572</v>
       </c>
       <c r="D70" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>72</v>
       </c>
@@ -1967,10 +1980,10 @@
         <v>3000142572</v>
       </c>
       <c r="D71" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>73</v>
       </c>
@@ -1981,10 +1994,10 @@
         <v>3000142572</v>
       </c>
       <c r="D72" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>74</v>
       </c>
@@ -1995,10 +2008,10 @@
         <v>3000142572</v>
       </c>
       <c r="D73" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -2009,10 +2022,10 @@
         <v>3000142572</v>
       </c>
       <c r="D74" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>76</v>
       </c>
@@ -2023,10 +2036,10 @@
         <v>3000142572</v>
       </c>
       <c r="D75" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>77</v>
       </c>
@@ -2037,10 +2050,10 @@
         <v>3000142572</v>
       </c>
       <c r="D76" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>78</v>
       </c>
@@ -2051,10 +2064,10 @@
         <v>3000142572</v>
       </c>
       <c r="D77" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -2065,10 +2078,10 @@
         <v>3000142572</v>
       </c>
       <c r="D78" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>80</v>
       </c>
@@ -2079,10 +2092,10 @@
         <v>3000142572</v>
       </c>
       <c r="D79" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>81</v>
       </c>
@@ -2093,10 +2106,10 @@
         <v>3000142572</v>
       </c>
       <c r="D80" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>82</v>
       </c>
@@ -2107,10 +2120,10 @@
         <v>3000142572</v>
       </c>
       <c r="D81" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>83</v>
       </c>
@@ -2121,10 +2134,10 @@
         <v>3000142572</v>
       </c>
       <c r="D82" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>84</v>
       </c>
@@ -2135,10 +2148,10 @@
         <v>3000142572</v>
       </c>
       <c r="D83" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>85</v>
       </c>
@@ -2149,10 +2162,10 @@
         <v>3000142572</v>
       </c>
       <c r="D84" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>86</v>
       </c>
@@ -2163,10 +2176,10 @@
         <v>3000142572</v>
       </c>
       <c r="D85" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>87</v>
       </c>
@@ -2177,10 +2190,10 @@
         <v>3000142572</v>
       </c>
       <c r="D86" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>88</v>
       </c>
@@ -2191,10 +2204,10 @@
         <v>3000142572</v>
       </c>
       <c r="D87" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>89</v>
       </c>
@@ -2205,10 +2218,10 @@
         <v>3000142572</v>
       </c>
       <c r="D88" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>90</v>
       </c>
@@ -2219,10 +2232,10 @@
         <v>3000142572</v>
       </c>
       <c r="D89" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>91</v>
       </c>
@@ -2233,10 +2246,10 @@
         <v>3000142572</v>
       </c>
       <c r="D90" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>92</v>
       </c>
@@ -2247,10 +2260,10 @@
         <v>3000142572</v>
       </c>
       <c r="D91" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>93</v>
       </c>
@@ -2261,10 +2274,10 @@
         <v>3000142572</v>
       </c>
       <c r="D92" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>94</v>
       </c>
@@ -2275,10 +2288,10 @@
         <v>3000142572</v>
       </c>
       <c r="D93" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>95</v>
       </c>
@@ -2289,10 +2302,10 @@
         <v>3000142572</v>
       </c>
       <c r="D94" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>96</v>
       </c>
@@ -2303,10 +2316,10 @@
         <v>3000142572</v>
       </c>
       <c r="D95" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>97</v>
       </c>
@@ -2317,10 +2330,10 @@
         <v>3000142572</v>
       </c>
       <c r="D96" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>98</v>
       </c>
@@ -2331,7 +2344,7 @@
         <v>3000142572</v>
       </c>
       <c r="D97" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2345,7 +2358,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2357,7 +2370,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>